<commit_message>
MCMF with edge demands
하한값이 있는 간선 추가
</commit_message>
<xml_diff>
--- a/Allocation_Of_Manpower/police_info.xlsx
+++ b/Allocation_Of_Manpower/police_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive - dongguk.edu\DGU_Unv\2022\3-2학기\컴퓨터알고리즘과실습\팀 프로젝트\Allocation_Of_Manpower\Allocation_Of_Manpower\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dongguk0-my.sharepoint.com/personal/97mjh1012_dongguk_edu/Documents/DGU_Unv/2022/3-2학기/컴퓨터알고리즘과실습/팀 프로젝트/Allocation_Of_Manpower/Allocation_Of_Manpower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4756A98-0B94-46CF-B006-32A26ED271BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{C4756A98-0B94-46CF-B006-32A26ED271BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB186FF4-C7BF-4C50-9C77-F78CDC71785F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{4D429D74-AFE0-4EB6-B702-C2DE111D2850}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{4D429D74-AFE0-4EB6-B702-C2DE111D2850}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,49 +36,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>근무지명</t>
+    <t>office0</t>
+  </si>
+  <si>
+    <t>office1</t>
+  </si>
+  <si>
+    <t>region0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>관할 구역</t>
+    <t>region1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>동원 가능 인원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1, 2, 3, 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1, 4, 5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2, 3, 4, 5, 6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4, 5, 6</t>
+    <t>region2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -125,12 +99,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99F5866-2BE2-4A52-B86F-F8543FF590ED}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -457,59 +434,32 @@
     <col min="1" max="16384" width="16.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>40</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>65</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>